<commit_message>
Added a few Testing cases
</commit_message>
<xml_diff>
--- a/Progress 8 Dec 2015/2 - Testing.xlsx
+++ b/Progress 8 Dec 2015/2 - Testing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr date1904="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ananda\Documents\conferenceScheduler\Progress 8 Dec 2015\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Test Cases" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,17 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Test Cases</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>When deleting a reservation, a user will be prompted to make sure they really want to delete it.</t>
+  </si>
+  <si>
+    <t>Admins can assign users to themselves as managers</t>
+  </si>
+  <si>
+    <t>Admin manager assign page should display both admins and managers</t>
+  </si>
+  <si>
+    <t>A manager should be able to delete a user's reservation</t>
+  </si>
+  <si>
+    <t>An Admin can view/update/delete managers reservations as well</t>
+  </si>
+  <si>
+    <t>Users should not be able to make more than 10 reservations</t>
+  </si>
+  <si>
+    <t>A recurring reservation should be limited based on limit of reservations</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Anyone should be able to give a rating to a room that they had previously reserved</t>
+  </si>
+  <si>
+    <t>Anyone should be able to leave a comment on a room they previously reserved</t>
   </si>
 </sst>
 </file>
@@ -436,6 +463,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -461,15 +497,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -500,7 +527,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1">
+  <tableStyles count="1" defaultPivotStyle="PivotStyleMedium4">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1690,31 +1717,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV33"/>
+  <dimension ref="A1:IV41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="1" customWidth="1"/>
+    <col min="3" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" ht="28" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:4" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1728,8 +1755,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:4" ht="20.75" customHeight="1">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1740,8 +1767,8 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A4" s="16"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1750,8 +1777,8 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1760,8 +1787,8 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
@@ -1770,8 +1797,8 @@
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:4" ht="32.5" customHeight="1">
+      <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1780,8 +1807,8 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:4" ht="36">
+      <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
@@ -1792,8 +1819,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
@@ -1802,8 +1829,8 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:4" ht="32.5" customHeight="1">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1814,8 +1841,8 @@
       </c>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A11" s="16"/>
       <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
@@ -1824,8 +1851,8 @@
       </c>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
+    <row r="12" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A12" s="16"/>
       <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1836,8 +1863,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A13" s="16"/>
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
@@ -1846,8 +1873,8 @@
       </c>
       <c r="D13" s="11"/>
     </row>
-    <row r="14" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:4" ht="32.5" customHeight="1">
+      <c r="A14" s="16"/>
       <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1856,8 +1883,8 @@
       </c>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:4" ht="32.5" customHeight="1">
+      <c r="A15" s="16"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
@@ -1866,8 +1893,8 @@
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A16" s="16"/>
       <c r="B16" s="9" t="s">
         <v>20</v>
       </c>
@@ -1876,8 +1903,8 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1888,8 +1915,8 @@
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A18" s="16"/>
       <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1900,8 +1927,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+    <row r="19" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A19" s="16"/>
       <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1912,8 +1939,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
+    <row r="20" spans="1:4" ht="20.5" customHeight="1">
+      <c r="A20" s="16"/>
       <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1924,8 +1951,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:4" ht="12">
+      <c r="A21" s="16"/>
       <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
@@ -1934,101 +1961,159 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:4" ht="18" customHeight="1">
+      <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+    <row r="23" spans="1:4" ht="18" customHeight="1">
+      <c r="A23" s="23"/>
       <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" customHeight="1">
+      <c r="A24" s="23"/>
+      <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:4" ht="18" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+    <row r="26" spans="1:4" ht="18" customHeight="1">
+      <c r="A26" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B26" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="22" t="s">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:4" ht="18" customHeight="1">
+      <c r="A27" s="13"/>
+      <c r="B27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="18" customHeight="1">
+      <c r="A28" s="13"/>
+      <c r="B28" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" ht="18" customHeight="1">
+      <c r="A29" s="14"/>
+      <c r="B29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="22" t="s">
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:4" ht="18" customHeight="1">
+      <c r="A30" s="14"/>
+      <c r="B30" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="1:4" ht="18" customHeight="1">
+      <c r="A31" s="14"/>
+      <c r="B31" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-    </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:4" ht="18" customHeight="1">
+      <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="33" spans="1:2" ht="24">
+      <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+    <row r="34" spans="1:2" ht="18" customHeight="1">
+      <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
+    <row r="35" spans="1:2" ht="18" customHeight="1">
+      <c r="B35" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+    <row r="36" spans="1:2" ht="18" customHeight="1">
+      <c r="B36" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18" customHeight="1">
+      <c r="B37" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="24">
+      <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="39" spans="1:2" ht="24">
+      <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="18" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="18" customHeight="1">
+      <c r="B41" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A26:A31"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran through testing file
</commit_message>
<xml_diff>
--- a/Progress 8 Dec 2015/2 - Testing.xlsx
+++ b/Progress 8 Dec 2015/2 - Testing.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ananda\Documents\conferenceScheduler\Progress 8 Dec 2015\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Test Cases" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
   <si>
     <t>Test Cases</t>
   </si>
@@ -33,12 +38,6 @@
     <t>Test Case</t>
   </si>
   <si>
-    <t>Passed?</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Sign In</t>
   </si>
   <si>
@@ -105,12 +104,6 @@
     <t>Everyone can redirect to the page for searching for rooms/resources from dashboard</t>
   </si>
   <si>
-    <t>Passed Nov 18</t>
-  </si>
-  <si>
-    <t>Failed Nov 18</t>
-  </si>
-  <si>
     <t>Rejects, but no warning message shown</t>
   </si>
   <si>
@@ -141,9 +134,6 @@
     <t>Admins</t>
   </si>
   <si>
-    <t>Admins can assign perform the tasks of managers</t>
-  </si>
-  <si>
     <t>Admins can assign users to different managers</t>
   </si>
   <si>
@@ -186,9 +176,6 @@
     <t>An Admin can view/update/delete managers reservations as well</t>
   </si>
   <si>
-    <t>Users should not be able to make more than 10 reservations</t>
-  </si>
-  <si>
     <t>A recurring reservation should be limited based on limit of reservations</t>
   </si>
   <si>
@@ -199,6 +186,90 @@
   </si>
   <si>
     <t>Anyone should be able to leave a comment on a room they previously reserved</t>
+  </si>
+  <si>
+    <t>Reservations are made in blocks of 30 minutes</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Users can search for rooms by feature</t>
+  </si>
+  <si>
+    <t>Normal users cannot see the reservations of other users (only managers and admins can see this)</t>
+  </si>
+  <si>
+    <t>Users can change reservations</t>
+  </si>
+  <si>
+    <t>Monthly statements on usage (reservations made) are available to manager</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Forgotten passwords can be emailed to users</t>
+  </si>
+  <si>
+    <t>Monthly usage statements are emailed to manager</t>
+  </si>
+  <si>
+    <t>A manager can ONLY see and modify their users' reservations (not any other manager's users)</t>
+  </si>
+  <si>
+    <t>Admins can perform the tasks of managers and normal users</t>
+  </si>
+  <si>
+    <t>Waitlist</t>
+  </si>
+  <si>
+    <t>When you reserve a room that is not yet available, you are placed on a waitlist</t>
+  </si>
+  <si>
+    <t>A notification is provided when you get off the waitlist</t>
+  </si>
+  <si>
+    <t>Users should not be able to make more than 10 reservations (not including past reservations)</t>
+  </si>
+  <si>
+    <t>Should be able to reserve all or some of resources contained in room</t>
+  </si>
+  <si>
+    <t>Should be able to make recurring reservations (daily, weekly, monthly, or yearly)</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>November 18 Testing</t>
+  </si>
+  <si>
+    <t>December 8 Testing</t>
+  </si>
+  <si>
+    <t>November 18 Comments</t>
+  </si>
+  <si>
+    <t>December 8 Comments</t>
+  </si>
+  <si>
+    <t>No cancel button</t>
+  </si>
+  <si>
+    <t>Implementation is buggy</t>
+  </si>
+  <si>
+    <t>Some of the data is not correctly displayed</t>
+  </si>
+  <si>
+    <t>Not yet implemented</t>
+  </si>
+  <si>
+    <t>We haven't been able to get email to work</t>
   </si>
 </sst>
 </file>
@@ -426,7 +497,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -498,6 +569,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1717,23 +1791,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV41"/>
+  <dimension ref="A1:IV53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28" customHeight="1">
+    <row r="1" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1817,7 @@
       <c r="C1" s="20"/>
       <c r="D1" s="21"/>
     </row>
-    <row r="2" spans="1:4" ht="20.75" customHeight="1">
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1749,361 +1825,874 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.75" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" ht="32.5" customHeight="1">
+      <c r="E6" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="36">
+      <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20.5" customHeight="1">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="32.5" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>14</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="20.5" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" ht="32.5" customHeight="1">
+      <c r="E13" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" ht="32.5" customHeight="1">
+      <c r="E14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E15" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1">
-      <c r="A17" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="C17" s="7" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.5" customHeight="1">
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="12">
+        <v>29</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1">
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
       <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1">
+        <v>47</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
       <c r="B24" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" customHeight="1">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="18" customHeight="1">
-      <c r="A26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:4" ht="18" customHeight="1">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" ht="18" customHeight="1">
-      <c r="A28" s="13"/>
+        <v>58</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="23"/>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="B28" s="12" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1">
-      <c r="A29" s="14"/>
+      <c r="E28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
       <c r="B29" s="12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1">
-      <c r="A30" s="14"/>
+      <c r="E29" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
       <c r="B30" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" ht="18" customHeight="1">
+      <c r="E30" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
       <c r="B31" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:4" ht="18" customHeight="1">
-      <c r="A32" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
+      <c r="B32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:256" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:256" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="24">
-      <c r="B33" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="18" customHeight="1">
-      <c r="B34" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="18" customHeight="1">
-      <c r="B35" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="18" customHeight="1">
-      <c r="B36" s="1" t="s">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="12"/>
+      <c r="U46" s="12"/>
+      <c r="V46" s="12"/>
+      <c r="W46" s="12"/>
+      <c r="X46" s="12"/>
+      <c r="Y46" s="12"/>
+      <c r="Z46" s="12"/>
+      <c r="AA46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AD46" s="12"/>
+      <c r="AE46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AH46" s="12"/>
+      <c r="AI46" s="12"/>
+      <c r="AJ46" s="12"/>
+      <c r="AK46" s="12"/>
+      <c r="AL46" s="12"/>
+      <c r="AM46" s="12"/>
+      <c r="AN46" s="12"/>
+      <c r="AO46" s="12"/>
+      <c r="AP46" s="12"/>
+      <c r="AQ46" s="12"/>
+      <c r="AR46" s="12"/>
+      <c r="AS46" s="12"/>
+      <c r="AT46" s="12"/>
+      <c r="AU46" s="12"/>
+      <c r="AV46" s="12"/>
+      <c r="AW46" s="12"/>
+      <c r="AX46" s="12"/>
+      <c r="AY46" s="12"/>
+      <c r="AZ46" s="12"/>
+      <c r="BA46" s="12"/>
+      <c r="BB46" s="12"/>
+      <c r="BC46" s="12"/>
+      <c r="BD46" s="12"/>
+      <c r="BE46" s="12"/>
+      <c r="BF46" s="12"/>
+      <c r="BG46" s="12"/>
+      <c r="BH46" s="12"/>
+      <c r="BI46" s="12"/>
+      <c r="BJ46" s="12"/>
+      <c r="BK46" s="12"/>
+      <c r="BL46" s="12"/>
+      <c r="BM46" s="12"/>
+      <c r="BN46" s="12"/>
+      <c r="BO46" s="12"/>
+      <c r="BP46" s="12"/>
+      <c r="BQ46" s="12"/>
+      <c r="BR46" s="12"/>
+      <c r="BS46" s="12"/>
+      <c r="BT46" s="12"/>
+      <c r="BU46" s="12"/>
+      <c r="BV46" s="12"/>
+      <c r="BW46" s="12"/>
+      <c r="BX46" s="12"/>
+      <c r="BY46" s="12"/>
+      <c r="BZ46" s="12"/>
+      <c r="CA46" s="12"/>
+      <c r="CB46" s="12"/>
+      <c r="CC46" s="12"/>
+      <c r="CD46" s="12"/>
+      <c r="CE46" s="12"/>
+      <c r="CF46" s="12"/>
+      <c r="CG46" s="12"/>
+      <c r="CH46" s="12"/>
+      <c r="CI46" s="12"/>
+      <c r="CJ46" s="12"/>
+      <c r="CK46" s="12"/>
+      <c r="CL46" s="12"/>
+      <c r="CM46" s="12"/>
+      <c r="CN46" s="12"/>
+      <c r="CO46" s="12"/>
+      <c r="CP46" s="12"/>
+      <c r="CQ46" s="12"/>
+      <c r="CR46" s="12"/>
+      <c r="CS46" s="12"/>
+      <c r="CT46" s="12"/>
+      <c r="CU46" s="12"/>
+      <c r="CV46" s="12"/>
+      <c r="CW46" s="12"/>
+      <c r="CX46" s="12"/>
+      <c r="CY46" s="12"/>
+      <c r="CZ46" s="12"/>
+      <c r="DA46" s="12"/>
+      <c r="DB46" s="12"/>
+      <c r="DC46" s="12"/>
+      <c r="DD46" s="12"/>
+      <c r="DE46" s="12"/>
+      <c r="DF46" s="12"/>
+      <c r="DG46" s="12"/>
+      <c r="DH46" s="12"/>
+      <c r="DI46" s="12"/>
+      <c r="DJ46" s="12"/>
+      <c r="DK46" s="12"/>
+      <c r="DL46" s="12"/>
+      <c r="DM46" s="12"/>
+      <c r="DN46" s="12"/>
+      <c r="DO46" s="12"/>
+      <c r="DP46" s="12"/>
+      <c r="DQ46" s="12"/>
+      <c r="DR46" s="12"/>
+      <c r="DS46" s="12"/>
+      <c r="DT46" s="12"/>
+      <c r="DU46" s="12"/>
+      <c r="DV46" s="12"/>
+      <c r="DW46" s="12"/>
+      <c r="DX46" s="12"/>
+      <c r="DY46" s="12"/>
+      <c r="DZ46" s="12"/>
+      <c r="EA46" s="12"/>
+      <c r="EB46" s="12"/>
+      <c r="EC46" s="12"/>
+      <c r="ED46" s="12"/>
+      <c r="EE46" s="12"/>
+      <c r="EF46" s="12"/>
+      <c r="EG46" s="12"/>
+      <c r="EH46" s="12"/>
+      <c r="EI46" s="12"/>
+      <c r="EJ46" s="12"/>
+      <c r="EK46" s="12"/>
+      <c r="EL46" s="12"/>
+      <c r="EM46" s="12"/>
+      <c r="EN46" s="12"/>
+      <c r="EO46" s="12"/>
+      <c r="EP46" s="12"/>
+      <c r="EQ46" s="12"/>
+      <c r="ER46" s="12"/>
+      <c r="ES46" s="12"/>
+      <c r="ET46" s="12"/>
+      <c r="EU46" s="12"/>
+      <c r="EV46" s="12"/>
+      <c r="EW46" s="12"/>
+      <c r="EX46" s="12"/>
+      <c r="EY46" s="12"/>
+      <c r="EZ46" s="12"/>
+      <c r="FA46" s="12"/>
+      <c r="FB46" s="12"/>
+      <c r="FC46" s="12"/>
+      <c r="FD46" s="12"/>
+      <c r="FE46" s="12"/>
+      <c r="FF46" s="12"/>
+      <c r="FG46" s="12"/>
+      <c r="FH46" s="12"/>
+      <c r="FI46" s="12"/>
+      <c r="FJ46" s="12"/>
+      <c r="FK46" s="12"/>
+      <c r="FL46" s="12"/>
+      <c r="FM46" s="12"/>
+      <c r="FN46" s="12"/>
+      <c r="FO46" s="12"/>
+      <c r="FP46" s="12"/>
+      <c r="FQ46" s="12"/>
+      <c r="FR46" s="12"/>
+      <c r="FS46" s="12"/>
+      <c r="FT46" s="12"/>
+      <c r="FU46" s="12"/>
+      <c r="FV46" s="12"/>
+      <c r="FW46" s="12"/>
+      <c r="FX46" s="12"/>
+      <c r="FY46" s="12"/>
+      <c r="FZ46" s="12"/>
+      <c r="GA46" s="12"/>
+      <c r="GB46" s="12"/>
+      <c r="GC46" s="12"/>
+      <c r="GD46" s="12"/>
+      <c r="GE46" s="12"/>
+      <c r="GF46" s="12"/>
+      <c r="GG46" s="12"/>
+      <c r="GH46" s="12"/>
+      <c r="GI46" s="12"/>
+      <c r="GJ46" s="12"/>
+      <c r="GK46" s="12"/>
+      <c r="GL46" s="12"/>
+      <c r="GM46" s="12"/>
+      <c r="GN46" s="12"/>
+      <c r="GO46" s="12"/>
+      <c r="GP46" s="12"/>
+      <c r="GQ46" s="12"/>
+      <c r="GR46" s="12"/>
+      <c r="GS46" s="12"/>
+      <c r="GT46" s="12"/>
+      <c r="GU46" s="12"/>
+      <c r="GV46" s="12"/>
+      <c r="GW46" s="12"/>
+      <c r="GX46" s="12"/>
+      <c r="GY46" s="12"/>
+      <c r="GZ46" s="12"/>
+      <c r="HA46" s="12"/>
+      <c r="HB46" s="12"/>
+      <c r="HC46" s="12"/>
+      <c r="HD46" s="12"/>
+      <c r="HE46" s="12"/>
+      <c r="HF46" s="12"/>
+      <c r="HG46" s="12"/>
+      <c r="HH46" s="12"/>
+      <c r="HI46" s="12"/>
+      <c r="HJ46" s="12"/>
+      <c r="HK46" s="12"/>
+      <c r="HL46" s="12"/>
+      <c r="HM46" s="12"/>
+      <c r="HN46" s="12"/>
+      <c r="HO46" s="12"/>
+      <c r="HP46" s="12"/>
+      <c r="HQ46" s="12"/>
+      <c r="HR46" s="12"/>
+      <c r="HS46" s="12"/>
+      <c r="HT46" s="12"/>
+      <c r="HU46" s="12"/>
+      <c r="HV46" s="12"/>
+      <c r="HW46" s="12"/>
+      <c r="HX46" s="12"/>
+      <c r="HY46" s="12"/>
+      <c r="HZ46" s="12"/>
+      <c r="IA46" s="12"/>
+      <c r="IB46" s="12"/>
+      <c r="IC46" s="12"/>
+      <c r="ID46" s="12"/>
+      <c r="IE46" s="12"/>
+      <c r="IF46" s="12"/>
+      <c r="IG46" s="12"/>
+      <c r="IH46" s="12"/>
+      <c r="II46" s="12"/>
+      <c r="IJ46" s="12"/>
+      <c r="IK46" s="12"/>
+      <c r="IL46" s="12"/>
+      <c r="IM46" s="12"/>
+      <c r="IN46" s="12"/>
+      <c r="IO46" s="12"/>
+      <c r="IP46" s="12"/>
+      <c r="IQ46" s="12"/>
+      <c r="IR46" s="12"/>
+      <c r="IS46" s="12"/>
+      <c r="IT46" s="12"/>
+      <c r="IU46" s="12"/>
+      <c r="IV46" s="12"/>
+    </row>
+    <row r="47" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:256" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="18" customHeight="1">
-      <c r="B37" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="24">
-      <c r="B38" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="24">
-      <c r="A39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="18" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="18" customHeight="1">
-      <c r="B41" s="1" t="s">
-        <v>58</v>
+      <c r="E49" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A28:A33"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A22:A27"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>